<commit_message>
fixed issue #14 (error when importing work records with 0 hours)
</commit_message>
<xml_diff>
--- a/budgeteer-web-interface/src/test/resources/org/wickedsource/budgeteer/service/imports/testReport1.xlsx
+++ b/budgeteer-web-interface/src/test/resources/org/wickedsource/budgeteer/service/imports/testReport1.xlsx
@@ -17,26 +17,32 @@
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Arbeitspakete!$A$3:$M$3</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles" vbProcedure="false">'Arbeitspakete PM'!$1:$4</definedName>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Arbeitspakete PM'!$A$3:$G$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Titles" vbProcedure="false">'Aufwände gesamt'!$1:$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Titles" vbProcedure="false">'Aufwände gesamt'!$1:$4</definedName>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Aufwände gesamt'!$A$3:$J$3</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">Arbeitspakete!$1:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0" vbProcedure="false">Arbeitspakete!$1:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0" vbProcedure="false">Arbeitspakete!$1:$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0" vbProcedure="false">Arbeitspakete!$1:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Arbeitspakete!$A$3:$M$3</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Arbeitspakete!$A$3:$M$3</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Arbeitspakete!$A$3:$M$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Arbeitspakete!$A$3:$M$3</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles" vbProcedure="false">'Arbeitspakete PM'!$1:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0" vbProcedure="false">'Arbeitspakete PM'!$1:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0" vbProcedure="false">'Arbeitspakete PM'!$1:$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Titles_0_0_0" vbProcedure="false">'Arbeitspakete PM'!$1:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Arbeitspakete PM'!$A$3:$G$3</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Arbeitspakete PM'!$A$3:$G$3</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Arbeitspakete PM'!$A$3:$G$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Titles" vbProcedure="false">'Aufwände gesamt'!$1:$4</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Titles_0" vbProcedure="false">'Aufwände gesamt'!$1:$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Titles_0_0" vbProcedure="false">'Aufwände gesamt'!$1:$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Arbeitspakete PM'!$A$3:$G$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Titles" vbProcedure="false">'Aufwände gesamt'!$1:$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Titles_0" vbProcedure="false">'Aufwände gesamt'!$1:$4</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Titles_0_0" vbProcedure="false">'Aufwände gesamt'!$1:$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Titles_0_0_0" vbProcedure="false">'Aufwände gesamt'!$1:$4</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Aufwände gesamt'!$A$3:$J$3</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Aufwände gesamt'!$A$3:$J$3</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Aufwände gesamt'!$A$3:$J$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Aufwände gesamt'!$A$3:$J$3</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
@@ -421,15 +427,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>651960</xdr:colOff>
+      <xdr:colOff>678960</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>3600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>32760</xdr:colOff>
+      <xdr:colOff>59400</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>21600</xdr:rowOff>
+      <xdr:rowOff>21240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -444,8 +450,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12420720" y="3600"/>
-          <a:ext cx="2086200" cy="493920"/>
+          <a:off x="12447720" y="3600"/>
+          <a:ext cx="2085840" cy="493560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -465,15 +471,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>600120</xdr:colOff>
+      <xdr:colOff>627120</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>3600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1463400</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>23760</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>21600</xdr:rowOff>
+      <xdr:rowOff>21240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -488,8 +494,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7224840" y="3600"/>
-          <a:ext cx="2047680" cy="493920"/>
+          <a:off x="7251840" y="3600"/>
+          <a:ext cx="2047320" cy="493560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -509,15 +515,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>2330640</xdr:colOff>
+      <xdr:colOff>2357640</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>3600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>24840</xdr:colOff>
+      <xdr:colOff>51480</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>21600</xdr:rowOff>
+      <xdr:rowOff>21240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -532,8 +538,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10423080" y="3600"/>
-          <a:ext cx="2179080" cy="493920"/>
+          <a:off x="10450080" y="3600"/>
+          <a:ext cx="2178720" cy="493560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -559,7 +565,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="1" sqref="F4:F11 A1"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -972,7 +978,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D21" activeCellId="1" sqref="F4:F11 D21"/>
+      <selection pane="bottomLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1191,7 +1197,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F4" activeCellId="0" sqref="F4:F11"/>
+      <selection pane="bottomLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1337,7 +1343,7 @@
         <v>14</v>
       </c>
       <c r="H6" s="6" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>15</v>

</xml_diff>